<commit_message>
create new project locally
</commit_message>
<xml_diff>
--- a/first Task.xlsx
+++ b/first Task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evolvantsolutions-my.sharepoint.com/personal/mahmoud_arjoon_evolvant_tech/Documents/Documents/UiPath/Classic Ui Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{B154F0C5-32B8-4447-82E6-894D606C5D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D70A941E-4F8C-46F5-B88F-0A7B24E61187}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{B154F0C5-32B8-4447-82E6-894D606C5D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C69C9007-5833-468C-9097-151F28F43102}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15120" xr2:uid="{E1BD27E7-B3DE-4C0E-98F7-4AD66DEC8704}"/>
+    <workbookView xWindow="11355" yWindow="-14850" windowWidth="17595" windowHeight="10890" xr2:uid="{E1BD27E7-B3DE-4C0E-98F7-4AD66DEC8704}"/>
   </bookViews>
   <sheets>
     <sheet name="Joined Data" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>LastName</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>BookID</t>
-  </si>
-  <si>
-    <t>ID_1</t>
   </si>
   <si>
     <t>Sakir</t>
@@ -467,13 +464,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05E365C-8595-455F-9640-13D7AD63DF76}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="9" max="9" width="9.23046875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,185 +497,143 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2">
         <v>111200</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>5551098</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>989120</v>
       </c>
-      <c r="H2">
-        <v>111200</v>
-      </c>
-      <c r="I2">
-        <v>111200</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
       <c r="C3">
         <v>145443</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>5559876</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3">
         <v>285454</v>
       </c>
-      <c r="H3">
-        <v>145443</v>
-      </c>
-      <c r="I3">
-        <v>145443</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
       <c r="C4">
         <v>287556</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>5555432</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>873102</v>
       </c>
-      <c r="H4">
-        <v>287556</v>
-      </c>
-      <c r="I4">
-        <v>287556</v>
-      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5">
         <v>201485</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>5553210</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <v>832127</v>
       </c>
-      <c r="H5">
-        <v>201485</v>
-      </c>
-      <c r="I5">
-        <v>201485</v>
-      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
       <c r="C6">
         <v>287556</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>5555432</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6">
         <v>974320</v>
       </c>
-      <c r="H6">
-        <v>287556</v>
-      </c>
-      <c r="I6">
-        <v>287556</v>
-      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
       <c r="C7">
         <v>201485</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>5553210</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>890437</v>
-      </c>
-      <c r="H7">
-        <v>201485</v>
-      </c>
-      <c r="I7">
-        <v>201485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>